<commit_message>
Add vocaitonal school support
</commit_message>
<xml_diff>
--- a/学校代码.xlsx
+++ b/学校代码.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\编程\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\编程\中考报名\ExaminationOfHighSchoolEntranceInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25D94DA-DADE-433E-9E67-3E410A6BB7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C40968-7BD5-4B1A-96E7-9D6364E59528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{9D50F7C1-ECB6-4959-B305-99F98FD67CB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D50F7C1-ECB6-4959-B305-99F98FD67CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>南宁市第一中学(五象校区)</t>
   </si>
@@ -181,6 +181,90 @@
   </si>
   <si>
     <t>南宁市爱华学校友爱校区(民办)</t>
+  </si>
+  <si>
+    <t>南宁市第一职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市第三职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市第四职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市第六职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市卫生学校</t>
+  </si>
+  <si>
+    <t>广西南宁技师学院</t>
+  </si>
+  <si>
+    <t>南宁市体育运动学校</t>
+  </si>
+  <si>
+    <t>南宁市特殊教育学校</t>
+  </si>
+  <si>
+    <t>南宁信息工程职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市运德汽车运输职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁创艺艺术职业学校</t>
+  </si>
+  <si>
+    <t>南宁市南山艺术职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市电子工程学校</t>
+  </si>
+  <si>
+    <t>南宁市民族歌舞艺术职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市工贸职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市海纳商务职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁商贸学校</t>
+  </si>
+  <si>
+    <t>南宁市赛口职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市中南理工职业技术学校</t>
+  </si>
+  <si>
+    <t>广西演艺职业学院附属中等职业学校</t>
+  </si>
+  <si>
+    <t>广西经济职业学院附属中等职业学校</t>
+  </si>
+  <si>
+    <t>南宁市城市管理职业技术学校</t>
+  </si>
+  <si>
+    <t>南宁市绿腾健康管理职业技术学校</t>
+  </si>
+  <si>
+    <t>武鸣区职业技术学校</t>
+  </si>
+  <si>
+    <t>横州职业技术学校</t>
+  </si>
+  <si>
+    <t>宾阳县职业技术学校</t>
+  </si>
+  <si>
+    <t>上林县职业技术学校</t>
+  </si>
+  <si>
+    <t>马山县民族职业技术学校</t>
   </si>
 </sst>
 </file>
@@ -544,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141768EB-A07E-440D-AD6C-61E424B6AD46}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -971,6 +1055,230 @@
         <v>49</v>
       </c>
     </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>45010006</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>45010007</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>45010008</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>45010009</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>45010010</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>45010011</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>45010027</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>45010028</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>45010014</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>45010015</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>45010016</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>45010017</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>45010018</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>45010029</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>45010020</v>
+      </c>
+      <c r="B68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>45010030</v>
+      </c>
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>45010022</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>45010023</v>
+      </c>
+      <c r="B71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>45010024</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>45010025</v>
+      </c>
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>45010026</v>
+      </c>
+      <c r="B74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>45010031</v>
+      </c>
+      <c r="B75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>45010032</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>45010033</v>
+      </c>
+      <c r="B77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>45010034</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>45010035</v>
+      </c>
+      <c r="B79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>45010036</v>
+      </c>
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>45010037</v>
+      </c>
+      <c r="B81" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>